<commit_message>
stock sample files updated
</commit_message>
<xml_diff>
--- a/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
+++ b/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
@@ -13,52 +13,52 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
   <si>
-    <t>S_Name*</t>
-  </si>
-  <si>
-    <t>S_UniqueName</t>
-  </si>
-  <si>
-    <t>StockGroupUniqueName*</t>
-  </si>
-  <si>
-    <t>StockUnitCode*</t>
-  </si>
-  <si>
-    <t>OpeningAmount</t>
-  </si>
-  <si>
-    <t>OpeningQuantity</t>
-  </si>
-  <si>
-    <t>HSN_Number</t>
-  </si>
-  <si>
-    <t>TaxValue</t>
-  </si>
-  <si>
-    <t>TaxType</t>
-  </si>
-  <si>
-    <t>P_AccountUniqueName</t>
-  </si>
-  <si>
-    <t>P_Rate</t>
-  </si>
-  <si>
-    <t>P_StockUnitCode</t>
-  </si>
-  <si>
-    <t>S_AccountUniqueName</t>
-  </si>
-  <si>
-    <t>S_Rate</t>
-  </si>
-  <si>
-    <t>S_StockUnitCode</t>
-  </si>
-  <si>
-    <t>IsFsStock</t>
+    <t>stock name</t>
+  </si>
+  <si>
+    <t>stock unique name</t>
+  </si>
+  <si>
+    <t>stock group name/unique name</t>
+  </si>
+  <si>
+    <t>stock unit code*</t>
+  </si>
+  <si>
+    <t>opening amount</t>
+  </si>
+  <si>
+    <t>opening quantity</t>
+  </si>
+  <si>
+    <t>hsn number</t>
+  </si>
+  <si>
+    <t>sac number</t>
+  </si>
+  <si>
+    <t>tax value</t>
+  </si>
+  <si>
+    <t>tax type</t>
+  </si>
+  <si>
+    <t>purchase account name/unique name</t>
+  </si>
+  <si>
+    <t>purchase rate</t>
+  </si>
+  <si>
+    <t>purchase stock unit code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sales account name/unique name </t>
+  </si>
+  <si>
+    <t>sales rate</t>
+  </si>
+  <si>
+    <t>sales stock unit code</t>
   </si>
   <si>
     <t>Bed traction kit</t>
@@ -268,15 +268,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -315,11 +312,11 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -335,10 +332,10 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -356,7 +353,7 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -365,7 +362,7 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -374,619 +371,599 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="5"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="8">
+      <c r="D2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="7">
         <v>0.0</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>1.0</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7">
         <v>5.0</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="6">
         <v>1000.0</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="M2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="7">
+      <c r="O2" s="6">
         <v>1250.0</v>
       </c>
-      <c r="O2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
+      <c r="P2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="8">
+      <c r="D3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7">
         <v>0.0</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>0.0</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7">
         <v>5.0</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="7">
+      <c r="L3" s="6">
         <v>299.0</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="M3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="7">
+      <c r="O3" s="6">
         <v>399.0</v>
       </c>
-      <c r="O3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
+      <c r="P3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="D4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="7">
         <v>0.0</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>1.0</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7">
         <v>5.0</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="7">
+      <c r="L4" s="6">
         <v>360.0</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="M4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="7">
+      <c r="O4" s="6">
         <v>460.0</v>
       </c>
-      <c r="O4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P4" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
+      <c r="P4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="8">
+      <c r="D5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="7">
         <v>0.0</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>0.0</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7">
         <v>5.0</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="7">
+      <c r="L5" s="6">
         <v>150.0</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="M5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="7">
+      <c r="O5" s="6">
         <v>250.0</v>
       </c>
-      <c r="O5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P5" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
+      <c r="P5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="D6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="6">
         <v>1250.0</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>1.0</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>9.0211E7</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="8">
+      <c r="L6" s="7">
         <v>1000.0</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="M6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="O6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
+      <c r="P6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="D7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="6">
         <v>460.0</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>1.0</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>9.0211E7</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="J7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="K7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="8">
+      <c r="L7" s="7">
         <v>360.0</v>
       </c>
-      <c r="L7" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="M7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="O7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="O7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P7" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
+      <c r="P7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="D8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="6">
         <v>1400.0</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>1.0</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>9.0211E7</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="K8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="8">
+      <c r="L8" s="7">
         <v>1100.0</v>
       </c>
-      <c r="L8" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="M8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="O8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="O8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P8" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
+      <c r="P8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="D9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="6">
         <v>1900.0</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>2.0</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>9.0211E7</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="K9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="8">
+      <c r="L9" s="7">
         <v>550.0</v>
       </c>
-      <c r="L9" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="M9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="11" t="s">
+      <c r="O9" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P9" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
+      <c r="P9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="D10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="6">
         <v>5310.0</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="11">
         <v>9.0</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>9.0211E7</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7"/>
+      <c r="I10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="J10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="K10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="8">
+      <c r="L10" s="7">
         <v>450.0</v>
       </c>
-      <c r="L10" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="M10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="11" t="s">
+      <c r="O10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
+      <c r="P10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="7">
+      <c r="D11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="6">
         <v>150.0</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>1.0</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>9.0211E7</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="K11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="8">
+      <c r="L11" s="7">
         <v>80.0</v>
       </c>
-      <c r="L11" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="M11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="O11" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="O11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
+      <c r="P11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
sample file changes done for account and stock
</commit_message>
<xml_diff>
--- a/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
+++ b/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
@@ -216,7 +216,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -247,11 +247,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13.5"/>
+      <b val="true"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -265,6 +265,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -349,7 +355,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -362,8 +368,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -386,6 +392,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -400,12 +410,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -477,16 +487,13 @@
   </sheetPr>
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T4" activeCellId="0" sqref="T4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="48.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +685,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
@@ -725,7 +732,7 @@
       <c r="P4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="5"/>
+      <c r="Q4" s="9"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -795,7 +802,7 @@
       <c r="Z5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -835,7 +842,7 @@
       <c r="N6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="O6" s="11" t="s">
         <v>43</v>
       </c>
       <c r="P6" s="8" t="s">
@@ -853,7 +860,7 @@
       <c r="Z6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -893,7 +900,7 @@
       <c r="N7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="O7" s="11" t="s">
         <v>46</v>
       </c>
       <c r="P7" s="8" t="s">
@@ -911,7 +918,7 @@
       <c r="Z7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -951,7 +958,7 @@
       <c r="N8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="11" t="s">
         <v>50</v>
       </c>
       <c r="P8" s="8" t="s">
@@ -969,7 +976,7 @@
       <c r="Z8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1009,7 +1016,7 @@
       <c r="N9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O9" s="10" t="s">
+      <c r="O9" s="11" t="s">
         <v>54</v>
       </c>
       <c r="P9" s="8" t="s">
@@ -1027,7 +1034,7 @@
       <c r="Z9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1042,7 +1049,7 @@
       <c r="E10" s="7" t="n">
         <v>5310</v>
       </c>
-      <c r="F10" s="11" t="n">
+      <c r="F10" s="12" t="n">
         <v>9</v>
       </c>
       <c r="G10" s="8" t="n">
@@ -1067,7 +1074,7 @@
       <c r="N10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="O10" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P10" s="8" t="s">
@@ -1085,7 +1092,7 @@
       <c r="Z10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1125,7 +1132,7 @@
       <c r="N11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="O11" s="11" t="s">
         <v>61</v>
       </c>
       <c r="P11" s="8" t="s">

</xml_diff>

<commit_message>
Taxes and discount issues resolved
</commit_message>
<xml_diff>
--- a/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
+++ b/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
@@ -252,6 +252,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -271,6 +272,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -355,7 +357,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -372,24 +374,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -481,19 +479,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T4" activeCellId="0" sqref="T4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="ABA1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AMA6" activeCellId="0" sqref="AMA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="1" style="0" width="14.44"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="48.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="35.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,600 +555,534 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="5"/>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="8" t="n">
+      <c r="D2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8" t="n">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="7" t="n">
+      <c r="L2" s="5" t="n">
         <v>1000</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="7" t="n">
+      <c r="O2" s="5" t="n">
         <v>1250</v>
       </c>
-      <c r="P2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="5" t="s">
+      <c r="P2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="8" t="n">
+      <c r="D3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8" t="n">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="7" t="n">
+      <c r="L3" s="5" t="n">
         <v>299</v>
       </c>
-      <c r="M3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="8" t="s">
+      <c r="M3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="7" t="n">
+      <c r="O3" s="5" t="n">
         <v>399</v>
       </c>
-      <c r="P3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
+      <c r="P3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="8" t="n">
+      <c r="D4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8" t="n">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="7" t="n">
+      <c r="L4" s="5" t="n">
         <v>360</v>
       </c>
-      <c r="M4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="8" t="s">
+      <c r="M4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="7" t="n">
+      <c r="O4" s="5" t="n">
         <v>460</v>
       </c>
-      <c r="P4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
+      <c r="P4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="8" t="n">
+      <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="8" t="n">
+      <c r="F5" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8" t="n">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="7" t="n">
+      <c r="L5" s="5" t="n">
         <v>150</v>
       </c>
-      <c r="M5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="8" t="s">
+      <c r="M5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="7" t="n">
+      <c r="O5" s="5" t="n">
         <v>250</v>
       </c>
-      <c r="P5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
+      <c r="P5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="7" t="n">
+      <c r="D6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5" t="n">
         <v>1250</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="8" t="n">
+      <c r="G6" s="6" t="n">
         <v>90211000</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="8" t="n">
+      <c r="L6" s="6" t="n">
         <v>1000</v>
       </c>
-      <c r="M6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="8" t="s">
+      <c r="M6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
+      <c r="P6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="7" t="n">
+      <c r="D7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="5" t="n">
         <v>460</v>
       </c>
-      <c r="F7" s="8" t="n">
+      <c r="F7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="8" t="n">
+      <c r="G7" s="6" t="n">
         <v>90211000</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="8" t="n">
+      <c r="L7" s="6" t="n">
         <v>360</v>
       </c>
-      <c r="M7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" s="8" t="s">
+      <c r="M7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="O7" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="P7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
+      <c r="P7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+    <row r="8" customFormat="false" ht="35.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="7" t="n">
+      <c r="D8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="5" t="n">
         <v>1400</v>
       </c>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="8" t="n">
+      <c r="G8" s="6" t="n">
         <v>90211000</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="8" t="n">
+      <c r="L8" s="6" t="n">
         <v>1100</v>
       </c>
-      <c r="M8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="8" t="s">
+      <c r="M8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="P8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
+      <c r="P8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="7" t="n">
+      <c r="D9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="5" t="n">
         <v>1900</v>
       </c>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="8" t="n">
+      <c r="G9" s="6" t="n">
         <v>90211000</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8" t="s">
+      <c r="H9" s="6"/>
+      <c r="I9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="8" t="n">
+      <c r="L9" s="6" t="n">
         <v>550</v>
       </c>
-      <c r="M9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="8" t="s">
+      <c r="M9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O9" s="11" t="s">
+      <c r="O9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="P9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
+      <c r="P9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="7" t="n">
+      <c r="D10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="5" t="n">
         <v>5310</v>
       </c>
-      <c r="F10" s="12" t="n">
+      <c r="F10" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="G10" s="8" t="n">
+      <c r="G10" s="6" t="n">
         <v>90211000</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8" t="s">
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="8" t="n">
+      <c r="L10" s="6" t="n">
         <v>450</v>
       </c>
-      <c r="M10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" s="8" t="s">
+      <c r="M10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="11" t="s">
+      <c r="O10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="P10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
+      <c r="P10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+    <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="7" t="n">
+      <c r="D11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="5" t="n">
         <v>150</v>
       </c>
-      <c r="F11" s="8" t="n">
+      <c r="F11" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="8" t="n">
+      <c r="G11" s="6" t="n">
         <v>90211000</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8" t="s">
+      <c r="H11" s="6"/>
+      <c r="I11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="8" t="n">
+      <c r="L11" s="6" t="n">
         <v>80</v>
       </c>
-      <c r="M11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" s="8" t="s">
+      <c r="M11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="11" t="s">
+      <c r="O11" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="P11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
+      <c r="P11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fix: Blank file is being downloaded when user download sample excel file from import inventory
</commit_message>
<xml_diff>
--- a/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
+++ b/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prate\OneDrive\Desktop\MANSI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -22,256 +26,231 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="62">
   <si>
-    <t xml:space="preserve">stock name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stock unique name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stock group name/unique name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stock unit code*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opening amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opening quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hsn number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sac number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purchase account name/unique name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purchase rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purchase stock unit code</t>
+    <t>stock name</t>
+  </si>
+  <si>
+    <t>stock unique name</t>
+  </si>
+  <si>
+    <t>stock group name/unique name</t>
+  </si>
+  <si>
+    <t>stock unit code*</t>
+  </si>
+  <si>
+    <t>opening amount</t>
+  </si>
+  <si>
+    <t>opening quantity</t>
+  </si>
+  <si>
+    <t>hsn number</t>
+  </si>
+  <si>
+    <t>sac number</t>
+  </si>
+  <si>
+    <t>tax value</t>
+  </si>
+  <si>
+    <t>tax type</t>
+  </si>
+  <si>
+    <t>purchase account name/unique name</t>
+  </si>
+  <si>
+    <t>purchase rate</t>
+  </si>
+  <si>
+    <t>purchase stock unit code</t>
   </si>
   <si>
     <t xml:space="preserve">sales account name/unique name </t>
   </si>
   <si>
-    <t xml:space="preserve">sales rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sales stock unit code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customField1Heading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customField1Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customField2Heading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customField2Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bed traction kit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maingroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purchases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StockQualtiy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stock Quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arm sling pouch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">armslingpouch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cockup splint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cockupsplint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cervical collar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cervicalcollar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bed traction kit -Universal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bedtractionkituniversal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GST, INPUTGST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cockup splint-XLarge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cockupsplintxlarge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">460</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knee immobilizer-XLarge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kneeimmobilizerxlarge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foot drop splint right-Large</t>
-  </si>
-  <si>
-    <t xml:space="preserve">footdropsplintrightlarge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">950</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ankle support-Universal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anklesupportuniversal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">590</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shoulder pully</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shoulderpully</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150</t>
+    <t>sales rate</t>
+  </si>
+  <si>
+    <t>sales stock unit code</t>
+  </si>
+  <si>
+    <t>customField1Heading</t>
+  </si>
+  <si>
+    <t>customField1Value</t>
+  </si>
+  <si>
+    <t>customField2Heading</t>
+  </si>
+  <si>
+    <t>customField2Value</t>
+  </si>
+  <si>
+    <t>Bed traction kit</t>
+  </si>
+  <si>
+    <t>new11</t>
+  </si>
+  <si>
+    <t>maingroup</t>
+  </si>
+  <si>
+    <t>nos</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>purchases</t>
+  </si>
+  <si>
+    <t>sales</t>
+  </si>
+  <si>
+    <t>StockQualtiy</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Stock Quantity</t>
+  </si>
+  <si>
+    <t>Fine</t>
+  </si>
+  <si>
+    <t>Arm sling pouch</t>
+  </si>
+  <si>
+    <t>armslingpouch</t>
+  </si>
+  <si>
+    <t>Cockup splint</t>
+  </si>
+  <si>
+    <t>cockupsplint</t>
+  </si>
+  <si>
+    <t>Cervical collar</t>
+  </si>
+  <si>
+    <t>cervicalcollar</t>
+  </si>
+  <si>
+    <t>Bed traction kit -Universal</t>
+  </si>
+  <si>
+    <t>bedtractionkituniversal</t>
+  </si>
+  <si>
+    <t>Group1</t>
+  </si>
+  <si>
+    <t>5,12</t>
+  </si>
+  <si>
+    <t>GST, INPUTGST</t>
+  </si>
+  <si>
+    <t>1250</t>
+  </si>
+  <si>
+    <t>Cockup splint-XLarge</t>
+  </si>
+  <si>
+    <t>cockupsplintxlarge</t>
+  </si>
+  <si>
+    <t>460</t>
+  </si>
+  <si>
+    <t>Knee immobilizer-XLarge</t>
+  </si>
+  <si>
+    <t>kneeimmobilizerxlarge</t>
+  </si>
+  <si>
+    <t>5,18</t>
+  </si>
+  <si>
+    <t>1400</t>
+  </si>
+  <si>
+    <t>Foot drop splint right-Large</t>
+  </si>
+  <si>
+    <t>footdropsplintrightlarge</t>
+  </si>
+  <si>
+    <t>Group2</t>
+  </si>
+  <si>
+    <t>950</t>
+  </si>
+  <si>
+    <t>Ankle support-Universal</t>
+  </si>
+  <si>
+    <t>anklesupportuniversal</t>
+  </si>
+  <si>
+    <t>5,28</t>
+  </si>
+  <si>
+    <t>590</t>
+  </si>
+  <si>
+    <t>Shoulder pully</t>
+  </si>
+  <si>
+    <t>shoulderpully</t>
+  </si>
+  <si>
+    <t>150</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="13.5"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -296,125 +275,106 @@
     </fill>
   </fills>
   <borders count="5">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -473,28 +433,300 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="ABA1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AMA6" activeCellId="0" sqref="AMA6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="1" style="0" width="14.44"/>
+    <col min="1" max="20" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -569,17 +801,17 @@
       <c r="D2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="6">
         <v>0</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="6">
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>24</v>
       </c>
       <c r="H2" s="6"/>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="6">
         <v>5</v>
       </c>
       <c r="J2" s="6" t="s">
@@ -588,7 +820,7 @@
       <c r="K2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="5" t="n">
+      <c r="L2" s="5">
         <v>1000</v>
       </c>
       <c r="M2" s="6" t="s">
@@ -597,7 +829,7 @@
       <c r="N2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="5" t="n">
+      <c r="O2" s="5">
         <v>1250</v>
       </c>
       <c r="P2" s="6" t="s">
@@ -616,7 +848,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -629,17 +861,17 @@
       <c r="D3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="6">
         <v>0</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="6">
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="6"/>
-      <c r="I3" s="6" t="n">
+      <c r="I3" s="6">
         <v>5</v>
       </c>
       <c r="J3" s="6" t="s">
@@ -648,7 +880,7 @@
       <c r="K3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="5" t="n">
+      <c r="L3" s="5">
         <v>299</v>
       </c>
       <c r="M3" s="6" t="s">
@@ -657,7 +889,7 @@
       <c r="N3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="5" t="n">
+      <c r="O3" s="5">
         <v>399</v>
       </c>
       <c r="P3" s="6" t="s">
@@ -668,7 +900,7 @@
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -681,17 +913,17 @@
       <c r="D4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="6">
         <v>0</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="6">
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="6">
         <v>5</v>
       </c>
       <c r="J4" s="6" t="s">
@@ -700,7 +932,7 @@
       <c r="K4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L4" s="5">
         <v>360</v>
       </c>
       <c r="M4" s="6" t="s">
@@ -709,7 +941,7 @@
       <c r="N4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="5" t="n">
+      <c r="O4" s="5">
         <v>460</v>
       </c>
       <c r="P4" s="6" t="s">
@@ -720,7 +952,7 @@
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
@@ -733,17 +965,17 @@
       <c r="D5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="6">
         <v>0</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="6">
         <v>0</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="6">
         <v>5</v>
       </c>
       <c r="J5" s="6" t="s">
@@ -752,7 +984,7 @@
       <c r="K5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="5">
         <v>150</v>
       </c>
       <c r="M5" s="6" t="s">
@@ -761,7 +993,7 @@
       <c r="N5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="5" t="n">
+      <c r="O5" s="5">
         <v>250</v>
       </c>
       <c r="P5" s="6" t="s">
@@ -772,7 +1004,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
@@ -785,13 +1017,13 @@
       <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="5">
         <v>1250</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="6">
         <v>1</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="6">
         <v>90211000</v>
       </c>
       <c r="H6" s="6"/>
@@ -804,7 +1036,7 @@
       <c r="K6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="6" t="n">
+      <c r="L6" s="6">
         <v>1000</v>
       </c>
       <c r="M6" s="6" t="s">
@@ -824,7 +1056,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>44</v>
       </c>
@@ -837,13 +1069,13 @@
       <c r="D7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="5">
         <v>460</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="6">
         <v>1</v>
       </c>
-      <c r="G7" s="6" t="n">
+      <c r="G7" s="6">
         <v>90211000</v>
       </c>
       <c r="H7" s="6"/>
@@ -856,7 +1088,7 @@
       <c r="K7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="6" t="n">
+      <c r="L7" s="6">
         <v>360</v>
       </c>
       <c r="M7" s="6" t="s">
@@ -876,7 +1108,7 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="35.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:20" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>47</v>
       </c>
@@ -889,13 +1121,13 @@
       <c r="D8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="5">
         <v>1400</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="6">
         <v>1</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="6">
         <v>90211000</v>
       </c>
       <c r="H8" s="6"/>
@@ -908,7 +1140,7 @@
       <c r="K8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="6" t="n">
+      <c r="L8" s="6">
         <v>1100</v>
       </c>
       <c r="M8" s="6" t="s">
@@ -928,7 +1160,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:20" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>51</v>
       </c>
@@ -941,13 +1173,13 @@
       <c r="D9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="5">
         <v>1900</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="6">
         <v>2</v>
       </c>
-      <c r="G9" s="6" t="n">
+      <c r="G9" s="6">
         <v>90211000</v>
       </c>
       <c r="H9" s="6"/>
@@ -960,7 +1192,7 @@
       <c r="K9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="6" t="n">
+      <c r="L9" s="6">
         <v>550</v>
       </c>
       <c r="M9" s="6" t="s">
@@ -980,7 +1212,7 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>55</v>
       </c>
@@ -993,13 +1225,13 @@
       <c r="D10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="5">
         <v>5310</v>
       </c>
-      <c r="F10" s="11" t="n">
+      <c r="F10" s="11">
         <v>9</v>
       </c>
-      <c r="G10" s="6" t="n">
+      <c r="G10" s="6">
         <v>90211000</v>
       </c>
       <c r="H10" s="6"/>
@@ -1012,7 +1244,7 @@
       <c r="K10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="6" t="n">
+      <c r="L10" s="6">
         <v>450</v>
       </c>
       <c r="M10" s="6" t="s">
@@ -1032,7 +1264,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>59</v>
       </c>
@@ -1045,13 +1277,13 @@
       <c r="D11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="5">
         <v>150</v>
       </c>
-      <c r="F11" s="6" t="n">
+      <c r="F11" s="6">
         <v>1</v>
       </c>
-      <c r="G11" s="6" t="n">
+      <c r="G11" s="6">
         <v>90211000</v>
       </c>
       <c r="H11" s="6"/>
@@ -1064,7 +1296,7 @@
       <c r="K11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="6" t="n">
+      <c r="L11" s="6">
         <v>80</v>
       </c>
       <c r="M11" s="6" t="s">
@@ -1085,12 +1317,7 @@
       <c r="T11" s="7"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: Reduce zoom level of excel file
</commit_message>
<xml_diff>
--- a/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
+++ b/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prate\OneDrive\Desktop\MANSI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prate\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -216,7 +216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -227,31 +227,25 @@
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="13.5"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -359,7 +353,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -719,7 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -900,7 +894,7 @@
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
     </row>
-    <row r="4" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -1318,6 +1312,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Update sample excel file for stock import to support SKU code
</commit_message>
<xml_diff>
--- a/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
+++ b/apps/web-giddh/src/assets/sample-files/stock-sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prate\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,16 +15,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
   <si>
     <t>stock name</t>
   </si>
@@ -210,13 +205,16 @@
   </si>
   <si>
     <t>150</t>
+  </si>
+  <si>
+    <t>sku code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -246,6 +244,16 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -329,10 +337,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -363,9 +372,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -711,16 +722,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="20" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -781,8 +794,11 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -841,8 +857,11 @@
       <c r="T2" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="U2" s="12">
+        <v>523523</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -894,7 +913,7 @@
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
     </row>
-    <row r="4" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -946,7 +965,7 @@
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
     </row>
-    <row r="5" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
@@ -998,7 +1017,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
@@ -1050,7 +1069,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
     </row>
-    <row r="7" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>44</v>
       </c>
@@ -1102,7 +1121,7 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
     </row>
-    <row r="8" spans="1:20" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>47</v>
       </c>
@@ -1154,7 +1173,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
     </row>
-    <row r="9" spans="1:20" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>51</v>
       </c>
@@ -1206,7 +1225,7 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
     </row>
-    <row r="10" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>55</v>
       </c>
@@ -1258,7 +1277,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
     </row>
-    <row r="11" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>59</v>
       </c>

</xml_diff>